<commit_message>
when mapping to cdes search cde variables by pathology name and get latest version
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ErrorFiles/dementia_Niguarda_v3.xlsx
+++ b/src/main/resources/data/ErrorFiles/dementia_Niguarda_v3.xlsx
@@ -449,11 +449,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -488,12 +489,6 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -576,19 +571,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -596,11 +583,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -624,12 +619,12 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:M38"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,7 +786,7 @@
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>

</xml_diff>